<commit_message>
amended code to run .Rmd
</commit_message>
<xml_diff>
--- a/2020-10-16-retrofOrBust/tables.xlsx
+++ b/2020-10-16-retrofOrBust/tables.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ben/git.soton/serg/fridayfun/2020-10-16-retrofOrBust/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{944E8D71-1D42-6243-8807-1DE667C9239E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D4DFD-DA8B-8944-8C6E-5074D48A5AD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="1740" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B0C39530-95E7-654F-B562-BE55D2CA041E}"/>
+    <workbookView xWindow="0" yWindow="2900" windowWidth="28040" windowHeight="17440" xr2:uid="{B0C39530-95E7-654F-B562-BE55D2CA041E}"/>
   </bookViews>
   <sheets>
     <sheet name="Table1" sheetId="1" r:id="rId1"/>
     <sheet name="Table2" sheetId="2" r:id="rId2"/>
-    <sheet name="Table3" sheetId="3" r:id="rId3"/>
+    <sheet name="Table3.1" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>Energy Efficiency Rating band</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Modelled mean annual energy cost £)</t>
   </si>
   <si>
-    <t>Total modelled current energy cost</t>
-  </si>
-  <si>
     <t>A/B</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>                                24,172</t>
-  </si>
-  <si>
     <t>Social rented</t>
   </si>
   <si>
@@ -105,16 +99,48 @@
   </si>
   <si>
     <t>Grand total</t>
+  </si>
+  <si>
+    <t>Total modelled current energy cost (£)</t>
+  </si>
+  <si>
+    <r>
+      <t>Estimated upgrade cost</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (£)</t>
+    </r>
+  </si>
+  <si>
+    <t>Modelled post-upgrade annual energy cost (£)</t>
+  </si>
+  <si>
+    <t>Estimated total current energy costs/year £)</t>
+  </si>
+  <si>
+    <t>Estimated total retrofit costs (£)</t>
+  </si>
+  <si>
+    <t>Estimated annual energy cost reduction (%)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="6" formatCode="&quot;£&quot;#,##0_);[Red]\(&quot;£&quot;#,##0\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;£&quot;* #,##0.00_);_(&quot;£&quot;* \(#,##0.00\);_(&quot;£&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-[$£-809]* #,##0_-;\-[$£-809]* #,##0_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -124,6 +150,13 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -148,16 +181,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -470,13 +511,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4BB75A-A423-2742-AA25-C7A2A5EF3F06}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -489,101 +533,103 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>321</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="6">
         <v>396</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="4">
         <v>126965138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="3">
         <v>7969</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="6">
         <v>643</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <v>5122684312</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" s="3">
         <v>11909</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="6">
         <v>921</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <v>10972073425</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="3">
         <v>2936</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="6">
         <v>1391</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="4">
         <v>4082352013</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>832</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="6">
         <v>2008</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="4">
         <v>1671168272</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>206</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="6">
         <v>2988</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>614600298</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="7">
+        <f>SUM(B2:B7)</f>
+        <v>24173</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="4">
         <v>22589843457</v>
       </c>
     </row>
@@ -594,48 +640,191 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB699B7C-FA21-5A42-8939-EB3F9C595165}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>321</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="2">
+        <v>126965138</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3">
+        <v>7969</v>
+      </c>
+      <c r="C3" s="6">
+        <v>106360555149</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3303799648</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3">
+        <v>11909</v>
+      </c>
+      <c r="C4" s="6">
+        <v>158946026777</v>
+      </c>
+      <c r="D4" s="2">
+        <v>4937223452</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2936</v>
+      </c>
+      <c r="C5" s="6">
+        <v>39179368276</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1216999882</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>832</v>
+      </c>
+      <c r="C6" s="6">
+        <v>22379619319</v>
+      </c>
+      <c r="D6" s="2">
+        <v>428860094</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>206</v>
+      </c>
+      <c r="C7" s="6">
+        <v>5531617428</v>
+      </c>
+      <c r="D7" s="2">
+        <v>106002249</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3">
+        <v>24172</v>
+      </c>
+      <c r="C8" s="6">
+        <v>332397186950</v>
+      </c>
+      <c r="D8" s="2">
+        <v>10119850463</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{325E1EE0-D31E-544F-842C-2B490331AF82}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B2" s="3">
         <v>2279</v>
@@ -652,7 +841,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
         <v>1760</v>
@@ -669,7 +858,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <v>34</v>
@@ -686,7 +875,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3">
         <v>4073</v>
@@ -698,178 +887,182 @@
         <v>54825891515</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
+      <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>16</v>
+      <c r="B8" s="3">
+        <v>1566</v>
+      </c>
+      <c r="C8" s="2">
+        <v>519</v>
+      </c>
+      <c r="D8" s="2">
+        <v>813270738</v>
+      </c>
+      <c r="E8" s="2">
+        <v>20895338313</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3">
-        <v>1566</v>
+        <v>2983</v>
       </c>
       <c r="C9" s="2">
-        <v>519</v>
+        <v>1156</v>
       </c>
       <c r="D9" s="2">
-        <v>813270738</v>
+        <v>3448851991</v>
       </c>
       <c r="E9" s="2">
-        <v>20895338313</v>
+        <v>39818952169</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2983</v>
+        <v>17</v>
+      </c>
+      <c r="B10">
+        <v>256</v>
       </c>
       <c r="C10" s="2">
-        <v>1156</v>
+        <v>2498</v>
       </c>
       <c r="D10" s="2">
-        <v>3448851991</v>
+        <v>638827593</v>
       </c>
       <c r="E10" s="2">
-        <v>39818952169</v>
+        <v>6877231024</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3">
+        <v>4805</v>
+      </c>
+      <c r="D11" s="2">
+        <v>4900950321</v>
+      </c>
+      <c r="E11" s="2">
+        <v>67591521506</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
-        <v>256</v>
-      </c>
-      <c r="C11" s="2">
-        <v>2498</v>
-      </c>
-      <c r="D11" s="2">
-        <v>638827593</v>
-      </c>
-      <c r="E11" s="2">
-        <v>6877231024</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="3">
-        <v>4805</v>
-      </c>
-      <c r="D12" s="2">
-        <v>4900950321</v>
-      </c>
-      <c r="E12" s="2">
-        <v>67591521506</v>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="1" t="s">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>16</v>
+      <c r="B14" s="3">
+        <v>4445</v>
+      </c>
+      <c r="C14" s="2">
+        <v>519</v>
+      </c>
+      <c r="D14" s="2">
+        <v>2309072932</v>
+      </c>
+      <c r="E14" s="2">
+        <v>59326934907</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="3">
-        <v>4445</v>
+        <v>10101</v>
       </c>
       <c r="C15" s="2">
-        <v>519</v>
+        <v>1156</v>
       </c>
       <c r="D15" s="2">
-        <v>2309072932</v>
+        <v>11676587304</v>
       </c>
       <c r="E15" s="2">
-        <v>59326934907</v>
+        <v>134812822534</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3">
-        <v>10101</v>
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>748</v>
       </c>
       <c r="C16" s="2">
-        <v>1156</v>
+        <v>2498</v>
       </c>
       <c r="D16" s="2">
-        <v>11676587304</v>
+        <v>1868763108</v>
       </c>
       <c r="E16" s="2">
-        <v>134812822534</v>
+        <v>20117972007</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>748</v>
-      </c>
-      <c r="C17" s="2">
-        <v>2498</v>
+        <v>9</v>
+      </c>
+      <c r="B17" s="3">
+        <v>15294</v>
       </c>
       <c r="D17" s="2">
-        <v>1868763108</v>
+        <v>15854423345</v>
       </c>
       <c r="E17" s="2">
-        <v>20117972007</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3">
-        <v>15294</v>
-      </c>
-      <c r="D18" s="2">
-        <v>15854423345</v>
-      </c>
-      <c r="E18" s="2">
         <v>214257729448</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="3">
         <v>24172</v>
       </c>
-      <c r="E20" s="2">
+      <c r="D19" s="2">
+        <f>D17+D11+D5</f>
+        <v>24059160057</v>
+      </c>
+      <c r="E19" s="2">
         <v>336675142469</v>
       </c>
     </row>

</xml_diff>